<commit_message>
Adición de encabezado para el manuscrito
</commit_message>
<xml_diff>
--- a/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
+++ b/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="149">
-  <si>
-    <t>Asignatura:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
   <si>
     <t>Fecha:</t>
   </si>
@@ -513,13 +510,10 @@
     <t>Solicitud gráfica de recurso:</t>
   </si>
   <si>
-    <t>Fotografía</t>
-  </si>
-  <si>
-    <t>Horizontal</t>
-  </si>
-  <si>
-    <t>LE_07_05_CO_REC110</t>
+    <t>Área:</t>
+  </si>
+  <si>
+    <t>CN_08_01_REC10</t>
   </si>
 </sst>
 </file>
@@ -1450,24 +1444,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1525,6 +1501,12 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2373,7 +2355,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
@@ -2409,14 +2391,12 @@
     <row r="2" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="105"/>
+      <c r="F2" s="79" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="87"/>
-      <c r="F2" s="79" t="s">
-        <v>1</v>
       </c>
       <c r="G2" s="80"/>
       <c r="H2" s="56"/>
@@ -2426,12 +2406,10 @@
     <row r="3" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="88">
         <v>8</v>
       </c>
-      <c r="D3" s="89"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107"/>
       <c r="F3" s="81"/>
       <c r="G3" s="82"/>
       <c r="H3" s="56"/>
@@ -2441,17 +2419,15 @@
     <row r="4" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+        <v>54</v>
+      </c>
+      <c r="C4" s="106"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="5"/>
       <c r="F4" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G4" s="54"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
       <c r="J4" s="16"/>
@@ -2460,18 +2436,16 @@
     <row r="5" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="5"/>
       <c r="F5" s="53" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
-        <v>Motor del recurso</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>103</v>
-      </c>
+        <v/>
+      </c>
+      <c r="G5" s="53"/>
       <c r="H5" s="56"/>
       <c r="I5" s="77"/>
       <c r="J5" s="16"/>
@@ -2493,13 +2467,13 @@
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2515,7 +2489,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="83" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="84"/>
       <c r="H8" s="84"/>
@@ -2530,64 +2504,58 @@
     </row>
     <row r="9" spans="1:16" ht="26.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="24" t="s">
+      <c r="D9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="E9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="76" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="76" t="s">
-        <v>138</v>
-      </c>
-      <c r="J9" s="25" t="s">
+      <c r="K9" s="26" t="s">
         <v>7</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
-        <v>IMG01</v>
-      </c>
-      <c r="B10" s="27">
-        <v>187654</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B10" s="27"/>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Recurso F13</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>147</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_07_05_CO_REC110_IMG01.jpg</v>
+        <v/>
       </c>
       <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="H10" s="14" t="str">
         <f>IF(I10&lt;&gt;"",IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
@@ -5224,71 +5192,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
+      <c r="A1" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="90"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="47"/>
-      <c r="C2" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="99"/>
+      <c r="C2" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A3" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="47"/>
-      <c r="C3" s="103" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="105"/>
+      <c r="C3" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
       <c r="F3" s="48"/>
       <c r="H3" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="J3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="38" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A4" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="E4" s="45" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="48"/>
       <c r="H4" s="38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="38">
         <v>1</v>
@@ -5299,23 +5267,23 @@
     </row>
     <row r="5" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="106" t="str">
+        <v>35</v>
+      </c>
+      <c r="D5" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="107"/>
+      <c r="E5" s="101"/>
       <c r="F5" s="48"/>
       <c r="H5" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="38">
         <v>2</v>
@@ -5326,7 +5294,7 @@
     </row>
     <row r="6" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
@@ -5334,10 +5302,10 @@
       <c r="E6" s="47"/>
       <c r="F6" s="48"/>
       <c r="H6" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" s="38">
         <v>3</v>
@@ -5348,23 +5316,23 @@
     </row>
     <row r="7" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="92" t="str">
+        <v>143</v>
+      </c>
+      <c r="D7" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
       <c r="H7" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="38">
         <v>4</v>
@@ -5375,7 +5343,7 @@
     </row>
     <row r="8" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A8" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
@@ -5383,7 +5351,7 @@
       <c r="E8" s="47"/>
       <c r="F8" s="48"/>
       <c r="I8" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8" s="38">
         <v>5</v>
@@ -5394,7 +5362,7 @@
     </row>
     <row r="9" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A9" s="49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
@@ -5402,7 +5370,7 @@
       <c r="E9" s="47"/>
       <c r="F9" s="48"/>
       <c r="I9" s="38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="38">
         <v>6</v>
@@ -5413,7 +5381,7 @@
     </row>
     <row r="10" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5421,7 +5389,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="52"/>
       <c r="I10" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J10" s="38">
         <v>7</v>
@@ -5432,7 +5400,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="I11" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="38">
         <v>8</v>
@@ -5443,7 +5411,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I12" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="38">
         <v>9</v>
@@ -5453,16 +5421,16 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A13" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96"/>
+      <c r="A13" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
       <c r="I13" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" s="38">
         <v>10</v>
@@ -5479,7 +5447,7 @@
       <c r="E14" s="47"/>
       <c r="F14" s="48"/>
       <c r="I14" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J14" s="38">
         <v>11</v>
@@ -5490,15 +5458,15 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="47"/>
-      <c r="C15" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
+      <c r="C15" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="93"/>
       <c r="J15" s="38">
         <v>12</v>
       </c>
@@ -5508,20 +5476,20 @@
     </row>
     <row r="16" spans="1:11" ht="67.099999999999994" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="E16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="41" t="s">
-        <v>18</v>
-      </c>
       <c r="F16" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J16" s="38">
         <v>13</v>
@@ -5532,18 +5500,18 @@
     </row>
     <row r="17" spans="1:11" ht="32.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="100" t="str">
+        <v>35</v>
+      </c>
+      <c r="D17" s="94" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="96"/>
       <c r="J17" s="38">
         <v>14</v>
       </c>
@@ -5553,18 +5521,18 @@
     </row>
     <row r="18" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="78" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="92" t="str">
+        <v>144</v>
+      </c>
+      <c r="D18" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="93"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="87"/>
       <c r="J18" s="38">
         <v>15</v>
       </c>
@@ -5574,7 +5542,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -5593,7 +5561,7 @@
     </row>
     <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
@@ -5955,542 +5923,542 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A1" s="108" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="108" t="s">
+      <c r="A1" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="D1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="108" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="108" t="s">
+      <c r="F1" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="G1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="H1" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="109" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
       <c r="H2" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="J2" s="57" t="s">
         <v>67</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="C3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="D3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="E3" s="58" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>74</v>
       </c>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
       <c r="H3" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="60" t="s">
+      <c r="F4" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G4" s="60"/>
       <c r="H4" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I4" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>82</v>
-      </c>
       <c r="C5" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E5" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G5" s="62"/>
       <c r="H5" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="60" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="J6" s="60" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A7" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>86</v>
-      </c>
       <c r="C7" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E7" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I7" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J7" s="60"/>
     </row>
     <row r="8" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="60" t="s">
-        <v>88</v>
-      </c>
       <c r="C8" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E8" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I8" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J8" s="60"/>
     </row>
     <row r="9" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>90</v>
-      </c>
       <c r="C9" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E9" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I9" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J9" s="60"/>
     </row>
     <row r="10" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="C10" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="60" t="s">
         <v>92</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="60" t="s">
-        <v>93</v>
       </c>
       <c r="F10" s="60"/>
       <c r="G10" s="60"/>
       <c r="H10" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I10" s="60"/>
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A11" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="60" t="s">
-        <v>95</v>
-      </c>
       <c r="C11" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E11" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I11" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="60" t="s">
-        <v>97</v>
-      </c>
       <c r="C12" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E12" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="60" t="s">
         <v>79</v>
-      </c>
-      <c r="I12" s="60" t="s">
-        <v>80</v>
       </c>
       <c r="J12" s="60"/>
     </row>
     <row r="13" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A13" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="C13" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="64" t="s">
         <v>99</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>100</v>
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="63"/>
       <c r="H13" s="60"/>
       <c r="I13" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="63"/>
       <c r="K13" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="63" t="s">
-        <v>103</v>
-      </c>
       <c r="C14" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="64" t="s">
         <v>72</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>73</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="60"/>
       <c r="I14" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="63"/>
     </row>
     <row r="15" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A15" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="C15" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="60" t="s">
-        <v>106</v>
-      </c>
       <c r="D15" s="63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F15" s="63"/>
       <c r="G15" s="63"/>
       <c r="H15" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I15" s="63"/>
       <c r="J15" s="63"/>
       <c r="K15" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="95" x14ac:dyDescent="0.5">
       <c r="A16" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="65"/>
       <c r="C16" s="61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="64" t="s">
         <v>139</v>
-      </c>
-      <c r="F16" s="64" t="s">
-        <v>140</v>
       </c>
       <c r="G16" s="64"/>
       <c r="H16" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" s="65" t="s">
         <v>110</v>
-      </c>
-      <c r="I16" s="65" t="s">
-        <v>111</v>
       </c>
       <c r="J16" s="64"/>
       <c r="K16" s="66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A17" s="60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="60"/>
       <c r="C17" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="60" t="s">
-        <v>73</v>
-      </c>
       <c r="E17" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="60" t="s">
         <v>114</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>115</v>
       </c>
       <c r="G17" s="60"/>
       <c r="H17" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="67" t="s">
         <v>116</v>
-      </c>
-      <c r="I17" s="67" t="s">
-        <v>117</v>
       </c>
       <c r="J17" s="60"/>
       <c r="K17" s="68" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="70" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="C21" s="72" t="s">
         <v>121</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>122</v>
       </c>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="73" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="C22" s="75" t="s">
         <v>124</v>
-      </c>
-      <c r="C22" s="75" t="s">
-        <v>125</v>
       </c>
       <c r="D22" s="74"/>
       <c r="E22" s="74"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="C23" s="75" t="s">
         <v>127</v>
-      </c>
-      <c r="C23" s="75" t="s">
-        <v>128</v>
       </c>
       <c r="D23" s="74"/>
       <c r="E23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A24" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="C24" s="75" t="s">
         <v>130</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>131</v>
       </c>
       <c r="D24" s="74"/>
       <c r="E24" s="74"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="C25" s="75" t="s">
         <v>133</v>
-      </c>
-      <c r="C25" s="75" t="s">
-        <v>134</v>
       </c>
       <c r="D25" s="74"/>
       <c r="E25" s="74"/>
     </row>
     <row r="26" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A26" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="C26" s="75" t="s">
         <v>136</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>137</v>
       </c>
       <c r="D26" s="74"/>
       <c r="E26" s="74"/>

</xml_diff>

<commit_message>
Actualización de fórmulas en la Solicitud Gráfica
</commit_message>
<xml_diff>
--- a/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
+++ b/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="146">
   <si>
     <t>Fecha:</t>
   </si>
@@ -251,9 +251,6 @@
     <t>110 x 110 px</t>
   </si>
   <si>
-    <t>CI_S3_01_REC10_F1</t>
-  </si>
-  <si>
     <t>Test - con imagen</t>
   </si>
   <si>
@@ -263,12 +260,6 @@
     <t>500 x 500 px</t>
   </si>
   <si>
-    <t>CI_S3_01_REC10_F1n</t>
-  </si>
-  <si>
-    <t>CI_S3_01_REC10_F1a</t>
-  </si>
-  <si>
     <t>M6A</t>
   </si>
   <si>
@@ -276,9 +267,6 @@
   </si>
   <si>
     <t>Test matemático (fórmula)</t>
-  </si>
-  <si>
-    <t>CI_S3_01_REC10_F1r</t>
   </si>
   <si>
     <t>M8A</t>
@@ -400,12 +388,6 @@
     <t>JPG o PNG</t>
   </si>
   <si>
-    <t>CI_S3_01_CE_F1_small</t>
-  </si>
-  <si>
-    <t>CI_S3_01_CE_F1_zoom</t>
-  </si>
-  <si>
     <t>Las fotos pueden tener otras medidas pero menores y deben mantenerse dentro de estos ratios. Por ejemplo, si pones el mapa de Chile, que es muy vertical, su máximo de alto van a ser 600 (y su anchura serán por ejemplo, 100 px) en el caso del zoom.</t>
   </si>
   <si>
@@ -435,48 +417,18 @@
     <t>Asignatura</t>
   </si>
   <si>
-    <t>CI</t>
-  </si>
-  <si>
-    <t>Ciencias</t>
-  </si>
-  <si>
     <t>Nivel</t>
   </si>
   <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>3ero Secundaria</t>
-  </si>
-  <si>
     <t>Guión</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>Guión 1</t>
-  </si>
-  <si>
     <t>Cuaderno de estudio o Recurso</t>
   </si>
   <si>
-    <t>CE ó REC10</t>
-  </si>
-  <si>
-    <t>Cuaderno de estudio o Recurso número 10</t>
-  </si>
-  <si>
     <t>Foto</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Foto o imagen número 1</t>
-  </si>
-  <si>
     <t>Small o Zoom (CE); Normal, Ampliada o Respuesta (REC); cuando aplica</t>
   </si>
   <si>
@@ -514,6 +466,51 @@
   </si>
   <si>
     <t>CN_08_01_REC10</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01n</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01_small</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01a</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01r</t>
+  </si>
+  <si>
+    <t>CN_08_02_REC10_IMG01_zoom</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Octavo Básica Secundaria</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Guión 2</t>
+  </si>
+  <si>
+    <t>REC10</t>
+  </si>
+  <si>
+    <t>IMG01</t>
+  </si>
+  <si>
+    <t>Imagen número 1</t>
+  </si>
+  <si>
+    <t>Recurso número 10 (para el Cuaderno de Estudio no se escribe nada)</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1210,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1444,69 +1441,72 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2355,7 +2355,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:D5"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
@@ -2391,10 +2391,10 @@
     <row r="2" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="105"/>
+        <v>129</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="87"/>
       <c r="F2" s="79" t="s">
         <v>0</v>
       </c>
@@ -2408,8 +2408,8 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="107"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
       <c r="F3" s="81"/>
       <c r="G3" s="82"/>
       <c r="H3" s="56"/>
@@ -2421,8 +2421,8 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="107"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="5"/>
       <c r="F4" s="55" t="s">
         <v>55</v>
@@ -2438,8 +2438,8 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="5"/>
       <c r="F5" s="53" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2470,7 +2470,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>39</v>
@@ -2528,7 +2528,7 @@
         <v>60</v>
       </c>
       <c r="I9" s="76" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>6</v>
@@ -2558,11 +2558,11 @@
         <v/>
       </c>
       <c r="H10" s="14" t="str">
-        <f>IF(I10&lt;&gt;"",IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I10" s="14" t="str">
-        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J10" s="14"/>
@@ -2589,11 +2589,11 @@
         <v/>
       </c>
       <c r="H11" s="14" t="str">
-        <f t="shared" ref="H11:H74" si="2">IF(I11&lt;&gt;"",IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H11:H74" si="2">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I11" s="14" t="str">
-        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J11" s="19"/>
@@ -2624,7 +2624,7 @@
         <v/>
       </c>
       <c r="I12" s="14" t="str">
-        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J12" s="19"/>
@@ -2655,7 +2655,7 @@
         <v/>
       </c>
       <c r="I13" s="14" t="str">
-        <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J13" s="19"/>
@@ -2686,7 +2686,7 @@
         <v/>
       </c>
       <c r="I14" s="14" t="str">
-        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J14" s="19"/>
@@ -2717,7 +2717,7 @@
         <v/>
       </c>
       <c r="I15" s="14" t="str">
-        <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J15" s="21"/>
@@ -2748,7 +2748,7 @@
         <v/>
       </c>
       <c r="I16" s="14" t="str">
-        <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J16" s="34"/>
@@ -2779,7 +2779,7 @@
         <v/>
       </c>
       <c r="I17" s="14" t="str">
-        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J17" s="21"/>
@@ -2810,7 +2810,7 @@
         <v/>
       </c>
       <c r="I18" s="14" t="str">
-        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J18" s="21"/>
@@ -2841,7 +2841,7 @@
         <v/>
       </c>
       <c r="I19" s="14" t="str">
-        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J19" s="34"/>
@@ -2872,7 +2872,7 @@
         <v/>
       </c>
       <c r="I20" s="14" t="str">
-        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J20" s="19"/>
@@ -2903,7 +2903,7 @@
         <v/>
       </c>
       <c r="I21" s="14" t="str">
-        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J21" s="21"/>
@@ -2934,7 +2934,7 @@
         <v/>
       </c>
       <c r="I22" s="14" t="str">
-        <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J22" s="14"/>
@@ -2962,7 +2962,7 @@
         <v/>
       </c>
       <c r="I23" s="14" t="str">
-        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J23" s="19"/>
@@ -2990,7 +2990,7 @@
         <v/>
       </c>
       <c r="I24" s="14" t="str">
-        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J24" s="14"/>
@@ -3018,7 +3018,7 @@
         <v/>
       </c>
       <c r="I25" s="14" t="str">
-        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J25" s="14"/>
@@ -3046,7 +3046,7 @@
         <v/>
       </c>
       <c r="I26" s="14" t="str">
-        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J26" s="14"/>
@@ -3074,7 +3074,7 @@
         <v/>
       </c>
       <c r="I27" s="14" t="str">
-        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J27" s="19"/>
@@ -3102,7 +3102,7 @@
         <v/>
       </c>
       <c r="I28" s="14" t="str">
-        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J28" s="19"/>
@@ -3130,7 +3130,7 @@
         <v/>
       </c>
       <c r="I29" s="14" t="str">
-        <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J29" s="19"/>
@@ -3158,7 +3158,7 @@
         <v/>
       </c>
       <c r="I30" s="14" t="str">
-        <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J30" s="19"/>
@@ -3183,7 +3183,7 @@
         <v/>
       </c>
       <c r="I31" s="14" t="str">
-        <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J31" s="19"/>
@@ -3208,7 +3208,7 @@
         <v/>
       </c>
       <c r="I32" s="14" t="str">
-        <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J32" s="19"/>
@@ -3233,7 +3233,7 @@
         <v/>
       </c>
       <c r="I33" s="14" t="str">
-        <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J33" s="19"/>
@@ -3258,7 +3258,7 @@
         <v/>
       </c>
       <c r="I34" s="14" t="str">
-        <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J34" s="19"/>
@@ -3283,7 +3283,7 @@
         <v/>
       </c>
       <c r="I35" s="14" t="str">
-        <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J35" s="14"/>
@@ -3308,7 +3308,7 @@
         <v/>
       </c>
       <c r="I36" s="14" t="str">
-        <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J36" s="14"/>
@@ -3333,7 +3333,7 @@
         <v/>
       </c>
       <c r="I37" s="14" t="str">
-        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J37" s="22"/>
@@ -3358,7 +3358,7 @@
         <v/>
       </c>
       <c r="I38" s="14" t="str">
-        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J38" s="23"/>
@@ -3383,7 +3383,7 @@
         <v/>
       </c>
       <c r="I39" s="14" t="str">
-        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J39" s="14"/>
@@ -3408,7 +3408,7 @@
         <v/>
       </c>
       <c r="I40" s="14" t="str">
-        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J40" s="14"/>
@@ -3433,7 +3433,7 @@
         <v/>
       </c>
       <c r="I41" s="14" t="str">
-        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J41" s="14"/>
@@ -3458,7 +3458,7 @@
         <v/>
       </c>
       <c r="I42" s="14" t="str">
-        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J42" s="14"/>
@@ -3483,7 +3483,7 @@
         <v/>
       </c>
       <c r="I43" s="14" t="str">
-        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J43" s="14"/>
@@ -3508,7 +3508,7 @@
         <v/>
       </c>
       <c r="I44" s="14" t="str">
-        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J44" s="14"/>
@@ -3533,7 +3533,7 @@
         <v/>
       </c>
       <c r="I45" s="14" t="str">
-        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J45" s="14"/>
@@ -3558,7 +3558,7 @@
         <v/>
       </c>
       <c r="I46" s="14" t="str">
-        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B46&lt;&gt;"",J46&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J46" s="14"/>
@@ -3583,7 +3583,7 @@
         <v/>
       </c>
       <c r="I47" s="14" t="str">
-        <f>IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J47" s="14"/>
@@ -3608,7 +3608,7 @@
         <v/>
       </c>
       <c r="I48" s="14" t="str">
-        <f>IF(OR(B48&lt;&gt;"",J48&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B48&lt;&gt;"",J48&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J48" s="14"/>
@@ -3633,7 +3633,7 @@
         <v/>
       </c>
       <c r="I49" s="14" t="str">
-        <f>IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J49" s="14"/>
@@ -3658,7 +3658,7 @@
         <v/>
       </c>
       <c r="I50" s="14" t="str">
-        <f>IF(OR(B50&lt;&gt;"",J50&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B50&lt;&gt;"",J50&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J50" s="14"/>
@@ -3683,7 +3683,7 @@
         <v/>
       </c>
       <c r="I51" s="14" t="str">
-        <f>IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J51" s="14"/>
@@ -3708,7 +3708,7 @@
         <v/>
       </c>
       <c r="I52" s="14" t="str">
-        <f>IF(OR(B52&lt;&gt;"",J52&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B52&lt;&gt;"",J52&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J52" s="14"/>
@@ -3733,7 +3733,7 @@
         <v/>
       </c>
       <c r="I53" s="14" t="str">
-        <f>IF(OR(B53&lt;&gt;"",J53&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B53&lt;&gt;"",J53&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J53" s="14"/>
@@ -3758,7 +3758,7 @@
         <v/>
       </c>
       <c r="I54" s="14" t="str">
-        <f>IF(OR(B54&lt;&gt;"",J54&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B54&lt;&gt;"",J54&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J54" s="14"/>
@@ -3783,7 +3783,7 @@
         <v/>
       </c>
       <c r="I55" s="14" t="str">
-        <f>IF(OR(B55&lt;&gt;"",J55&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B55&lt;&gt;"",J55&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J55" s="14"/>
@@ -3808,7 +3808,7 @@
         <v/>
       </c>
       <c r="I56" s="14" t="str">
-        <f>IF(OR(B56&lt;&gt;"",J56&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B56&lt;&gt;"",J56&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J56" s="14"/>
@@ -3833,7 +3833,7 @@
         <v/>
       </c>
       <c r="I57" s="14" t="str">
-        <f>IF(OR(B57&lt;&gt;"",J57&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B57&lt;&gt;"",J57&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J57" s="14"/>
@@ -3858,7 +3858,7 @@
         <v/>
       </c>
       <c r="I58" s="14" t="str">
-        <f>IF(OR(B58&lt;&gt;"",J58&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B58&lt;&gt;"",J58&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J58" s="14"/>
@@ -3883,7 +3883,7 @@
         <v/>
       </c>
       <c r="I59" s="14" t="str">
-        <f>IF(OR(B59&lt;&gt;"",J59&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B59&lt;&gt;"",J59&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J59" s="14"/>
@@ -3908,7 +3908,7 @@
         <v/>
       </c>
       <c r="I60" s="14" t="str">
-        <f>IF(OR(B60&lt;&gt;"",J60&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B60&lt;&gt;"",J60&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J60" s="14"/>
@@ -3933,7 +3933,7 @@
         <v/>
       </c>
       <c r="I61" s="14" t="str">
-        <f>IF(OR(B61&lt;&gt;"",J61&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B61&lt;&gt;"",J61&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J61" s="14"/>
@@ -3958,7 +3958,7 @@
         <v/>
       </c>
       <c r="I62" s="14" t="str">
-        <f>IF(OR(B62&lt;&gt;"",J62&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B62&lt;&gt;"",J62&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J62" s="14"/>
@@ -3983,7 +3983,7 @@
         <v/>
       </c>
       <c r="I63" s="14" t="str">
-        <f>IF(OR(B63&lt;&gt;"",J63&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B63&lt;&gt;"",J63&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J63" s="14"/>
@@ -4008,7 +4008,7 @@
         <v/>
       </c>
       <c r="I64" s="14" t="str">
-        <f>IF(OR(B64&lt;&gt;"",J64&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B64&lt;&gt;"",J64&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J64" s="14"/>
@@ -4033,7 +4033,7 @@
         <v/>
       </c>
       <c r="I65" s="14" t="str">
-        <f>IF(OR(B65&lt;&gt;"",J65&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B65&lt;&gt;"",J65&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J65" s="14"/>
@@ -4058,7 +4058,7 @@
         <v/>
       </c>
       <c r="I66" s="14" t="str">
-        <f>IF(OR(B66&lt;&gt;"",J66&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B66&lt;&gt;"",J66&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J66" s="14"/>
@@ -4083,7 +4083,7 @@
         <v/>
       </c>
       <c r="I67" s="14" t="str">
-        <f>IF(OR(B67&lt;&gt;"",J67&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B67&lt;&gt;"",J67&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J67" s="14"/>
@@ -4108,7 +4108,7 @@
         <v/>
       </c>
       <c r="I68" s="14" t="str">
-        <f>IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J68" s="14"/>
@@ -4133,7 +4133,7 @@
         <v/>
       </c>
       <c r="I69" s="14" t="str">
-        <f>IF(OR(B69&lt;&gt;"",J69&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B69&lt;&gt;"",J69&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J69" s="14"/>
@@ -4158,7 +4158,7 @@
         <v/>
       </c>
       <c r="I70" s="14" t="str">
-        <f>IF(OR(B70&lt;&gt;"",J70&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B70&lt;&gt;"",J70&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J70" s="14"/>
@@ -4183,7 +4183,7 @@
         <v/>
       </c>
       <c r="I71" s="14" t="str">
-        <f>IF(OR(B71&lt;&gt;"",J71&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B71&lt;&gt;"",J71&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J71" s="14"/>
@@ -4208,7 +4208,7 @@
         <v/>
       </c>
       <c r="I72" s="14" t="str">
-        <f>IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J72" s="14"/>
@@ -4233,7 +4233,7 @@
         <v/>
       </c>
       <c r="I73" s="14" t="str">
-        <f>IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J73" s="14"/>
@@ -4258,7 +4258,7 @@
         <v/>
       </c>
       <c r="I74" s="14" t="str">
-        <f>IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J74" s="14"/>
@@ -4279,11 +4279,11 @@
         <v/>
       </c>
       <c r="H75" s="14" t="str">
-        <f t="shared" ref="H75:H108" si="5">IF(I75&lt;&gt;"",IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H75:H108" si="5">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I75" s="14" t="str">
-        <f>IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J75" s="14"/>
@@ -4308,7 +4308,7 @@
         <v/>
       </c>
       <c r="I76" s="14" t="str">
-        <f>IF(OR(B76&lt;&gt;"",J76&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B76&lt;&gt;"",J76&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J76" s="14"/>
@@ -4333,7 +4333,7 @@
         <v/>
       </c>
       <c r="I77" s="14" t="str">
-        <f>IF(OR(B77&lt;&gt;"",J77&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B77&lt;&gt;"",J77&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J77" s="14"/>
@@ -4358,7 +4358,7 @@
         <v/>
       </c>
       <c r="I78" s="14" t="str">
-        <f>IF(OR(B78&lt;&gt;"",J78&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B78&lt;&gt;"",J78&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J78" s="14"/>
@@ -4383,7 +4383,7 @@
         <v/>
       </c>
       <c r="I79" s="14" t="str">
-        <f>IF(OR(B79&lt;&gt;"",J79&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B79&lt;&gt;"",J79&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J79" s="14"/>
@@ -4408,7 +4408,7 @@
         <v/>
       </c>
       <c r="I80" s="14" t="str">
-        <f>IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J80" s="14"/>
@@ -4433,7 +4433,7 @@
         <v/>
       </c>
       <c r="I81" s="14" t="str">
-        <f>IF(OR(B81&lt;&gt;"",J81&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B81&lt;&gt;"",J81&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J81" s="14"/>
@@ -4458,7 +4458,7 @@
         <v/>
       </c>
       <c r="I82" s="14" t="str">
-        <f>IF(OR(B82&lt;&gt;"",J82&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B82&lt;&gt;"",J82&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J82" s="14"/>
@@ -4483,7 +4483,7 @@
         <v/>
       </c>
       <c r="I83" s="14" t="str">
-        <f>IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J83" s="14"/>
@@ -4508,7 +4508,7 @@
         <v/>
       </c>
       <c r="I84" s="14" t="str">
-        <f>IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J84" s="14"/>
@@ -4533,7 +4533,7 @@
         <v/>
       </c>
       <c r="I85" s="14" t="str">
-        <f>IF(OR(B85&lt;&gt;"",J85&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B85&lt;&gt;"",J85&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J85" s="14"/>
@@ -4558,7 +4558,7 @@
         <v/>
       </c>
       <c r="I86" s="14" t="str">
-        <f>IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J86" s="14"/>
@@ -4583,7 +4583,7 @@
         <v/>
       </c>
       <c r="I87" s="14" t="str">
-        <f>IF(OR(B87&lt;&gt;"",J87&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B87&lt;&gt;"",J87&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J87" s="14"/>
@@ -4608,7 +4608,7 @@
         <v/>
       </c>
       <c r="I88" s="14" t="str">
-        <f>IF(OR(B88&lt;&gt;"",J88&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B88&lt;&gt;"",J88&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J88" s="14"/>
@@ -4633,7 +4633,7 @@
         <v/>
       </c>
       <c r="I89" s="14" t="str">
-        <f>IF(OR(B89&lt;&gt;"",J89&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B89&lt;&gt;"",J89&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J89" s="14"/>
@@ -4658,7 +4658,7 @@
         <v/>
       </c>
       <c r="I90" s="14" t="str">
-        <f>IF(OR(B90&lt;&gt;"",J90&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B90&lt;&gt;"",J90&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J90" s="14"/>
@@ -4683,7 +4683,7 @@
         <v/>
       </c>
       <c r="I91" s="14" t="str">
-        <f>IF(OR(B91&lt;&gt;"",J91&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B91&lt;&gt;"",J91&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J91" s="14"/>
@@ -4708,7 +4708,7 @@
         <v/>
       </c>
       <c r="I92" s="14" t="str">
-        <f>IF(OR(B92&lt;&gt;"",J92&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B92&lt;&gt;"",J92&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J92" s="14"/>
@@ -4733,7 +4733,7 @@
         <v/>
       </c>
       <c r="I93" s="14" t="str">
-        <f>IF(OR(B93&lt;&gt;"",J93&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B93&lt;&gt;"",J93&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J93" s="14"/>
@@ -4758,7 +4758,7 @@
         <v/>
       </c>
       <c r="I94" s="14" t="str">
-        <f>IF(OR(B94&lt;&gt;"",J94&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B94&lt;&gt;"",J94&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J94" s="14"/>
@@ -4783,7 +4783,7 @@
         <v/>
       </c>
       <c r="I95" s="14" t="str">
-        <f>IF(OR(B95&lt;&gt;"",J95&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B95&lt;&gt;"",J95&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J95" s="14"/>
@@ -4808,7 +4808,7 @@
         <v/>
       </c>
       <c r="I96" s="14" t="str">
-        <f>IF(OR(B96&lt;&gt;"",J96&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B96&lt;&gt;"",J96&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J96" s="14"/>
@@ -4833,7 +4833,7 @@
         <v/>
       </c>
       <c r="I97" s="14" t="str">
-        <f>IF(OR(B97&lt;&gt;"",J97&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B97&lt;&gt;"",J97&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J97" s="14"/>
@@ -4858,7 +4858,7 @@
         <v/>
       </c>
       <c r="I98" s="14" t="str">
-        <f>IF(OR(B98&lt;&gt;"",J98&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B98&lt;&gt;"",J98&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J98" s="14"/>
@@ -4883,7 +4883,7 @@
         <v/>
       </c>
       <c r="I99" s="14" t="str">
-        <f>IF(OR(B99&lt;&gt;"",J99&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B99&lt;&gt;"",J99&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J99" s="14"/>
@@ -4908,7 +4908,7 @@
         <v/>
       </c>
       <c r="I100" s="14" t="str">
-        <f>IF(OR(B100&lt;&gt;"",J100&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B100&lt;&gt;"",J100&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J100" s="14"/>
@@ -4933,7 +4933,7 @@
         <v/>
       </c>
       <c r="I101" s="14" t="str">
-        <f>IF(OR(B101&lt;&gt;"",J101&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B101&lt;&gt;"",J101&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J101" s="14"/>
@@ -4958,7 +4958,7 @@
         <v/>
       </c>
       <c r="I102" s="14" t="str">
-        <f>IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J102" s="14"/>
@@ -4983,7 +4983,7 @@
         <v/>
       </c>
       <c r="I103" s="14" t="str">
-        <f>IF(OR(B103&lt;&gt;"",J103&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B103&lt;&gt;"",J103&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J103" s="14"/>
@@ -5008,7 +5008,7 @@
         <v/>
       </c>
       <c r="I104" s="14" t="str">
-        <f>IF(OR(B104&lt;&gt;"",J104&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B104&lt;&gt;"",J104&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J104" s="14"/>
@@ -5033,7 +5033,7 @@
         <v/>
       </c>
       <c r="I105" s="14" t="str">
-        <f>IF(OR(B105&lt;&gt;"",J105&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B105&lt;&gt;"",J105&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J105" s="14"/>
@@ -5058,7 +5058,7 @@
         <v/>
       </c>
       <c r="I106" s="14" t="str">
-        <f>IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J106" s="14"/>
@@ -5083,7 +5083,7 @@
         <v/>
       </c>
       <c r="I107" s="14" t="str">
-        <f>IF(OR(B107&lt;&gt;"",J107&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B107&lt;&gt;"",J107&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J107" s="14"/>
@@ -5108,7 +5108,7 @@
         <v/>
       </c>
       <c r="I108" s="14" t="str">
-        <f>IF(OR(B108&lt;&gt;"",J108&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B108&lt;&gt;"",J108&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J108" s="14"/>
@@ -5192,25 +5192,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="90"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="46" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="47"/>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
       <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
@@ -5218,11 +5218,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="47"/>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="48"/>
       <c r="H3" s="38" t="s">
         <v>18</v>
@@ -5273,11 +5273,11 @@
       <c r="C5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="100" t="str">
+      <c r="D5" s="106" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="101"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="48"/>
       <c r="H5" s="38" t="s">
         <v>22</v>
@@ -5320,14 +5320,14 @@
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="78" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="86" t="str">
+        <v>127</v>
+      </c>
+      <c r="D7" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="H7" s="38" t="s">
         <v>24</v>
       </c>
@@ -5421,14 +5421,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="90"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
       <c r="I13" s="38" t="s">
         <v>33</v>
       </c>
@@ -5461,12 +5461,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="47"/>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="93"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
       <c r="J15" s="38">
         <v>12</v>
       </c>
@@ -5506,12 +5506,12 @@
       <c r="C17" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="94" t="str">
+      <c r="D17" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="95"/>
-      <c r="F17" s="96"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="J17" s="38">
         <v>14</v>
       </c>
@@ -5525,14 +5525,14 @@
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" s="86" t="str">
+        <v>128</v>
+      </c>
+      <c r="D18" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
       <c r="J18" s="38">
         <v>15</v>
       </c>
@@ -5903,8 +5903,8 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8125" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
@@ -5916,48 +5916,49 @@
     <col min="5" max="5" width="11.6875" style="38" customWidth="1"/>
     <col min="6" max="6" width="12.6875" style="38" customWidth="1"/>
     <col min="7" max="7" width="11" style="38" customWidth="1"/>
-    <col min="8" max="9" width="22.1875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="38" customWidth="1"/>
+    <col min="9" max="9" width="22.1875" style="38" customWidth="1"/>
     <col min="10" max="10" width="20.6875" style="38" customWidth="1"/>
     <col min="11" max="11" width="44.5" style="38" customWidth="1"/>
     <col min="12" max="16384" width="10.8125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
       <c r="H2" s="57" t="s">
         <v>65</v>
       </c>
@@ -5987,7 +5988,7 @@
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
       <c r="H3" s="58" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -5997,7 +5998,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="60" t="s">
         <v>71</v>
@@ -6006,26 +6007,26 @@
         <v>72</v>
       </c>
       <c r="E4" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G4" s="60"/>
       <c r="H4" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I4" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="61" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5" s="60" t="s">
         <v>71</v>
@@ -6034,17 +6035,17 @@
         <v>72</v>
       </c>
       <c r="E5" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G5" s="62"/>
       <c r="H5" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J5" s="62"/>
     </row>
@@ -6053,7 +6054,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C6" s="60" t="s">
         <v>71</v>
@@ -6062,30 +6063,30 @@
         <v>72</v>
       </c>
       <c r="E6" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G6" s="60" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A7" s="60" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>71</v>
@@ -6094,26 +6095,26 @@
         <v>72</v>
       </c>
       <c r="E7" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J7" s="60"/>
     </row>
     <row r="8" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="60" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C8" s="60" t="s">
         <v>71</v>
@@ -6122,26 +6123,26 @@
         <v>72</v>
       </c>
       <c r="E8" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J8" s="60"/>
     </row>
     <row r="9" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="60" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C9" s="60" t="s">
         <v>71</v>
@@ -6150,26 +6151,26 @@
         <v>72</v>
       </c>
       <c r="E9" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I9" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J9" s="60"/>
     </row>
     <row r="10" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="60" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C10" s="60" t="s">
         <v>71</v>
@@ -6178,22 +6179,24 @@
         <v>72</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F10" s="60"/>
       <c r="G10" s="60"/>
       <c r="H10" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="60"/>
+        <v>131</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>134</v>
+      </c>
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A11" s="60" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" s="60" t="s">
         <v>71</v>
@@ -6202,26 +6205,26 @@
         <v>72</v>
       </c>
       <c r="E11" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="60" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>71</v>
@@ -6230,53 +6233,53 @@
         <v>72</v>
       </c>
       <c r="E12" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="60" t="s">
         <v>76</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>77</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="60" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="I12" s="60" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="J12" s="60"/>
     </row>
     <row r="13" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A13" s="63" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C13" s="60" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="65" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G13" s="63"/>
       <c r="H13" s="60"/>
       <c r="I13" s="60" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="J13" s="63"/>
       <c r="K13" s="38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="63" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C14" s="60" t="s">
         <v>71</v>
@@ -6286,74 +6289,74 @@
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="65" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="60"/>
       <c r="I14" s="60" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="J14" s="63"/>
     </row>
     <row r="15" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A15" s="63" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C15" s="60" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F15" s="63"/>
       <c r="G15" s="63"/>
       <c r="H15" s="60" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="I15" s="63"/>
       <c r="J15" s="63"/>
       <c r="K15" s="38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="95" x14ac:dyDescent="0.5">
       <c r="A16" s="65" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B16" s="65"/>
       <c r="C16" s="61" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="G16" s="64"/>
       <c r="H16" s="65" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="I16" s="65" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="J16" s="64"/>
       <c r="K16" s="66" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A17" s="60" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B17" s="60"/>
       <c r="C17" s="60" t="s">
@@ -6363,102 +6366,102 @@
         <v>72</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G17" s="60"/>
       <c r="H17" s="67" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J17" s="60"/>
       <c r="K17" s="68" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="69" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="70" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="74" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="B22" s="110" t="s">
+        <v>138</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D22" s="74"/>
       <c r="E22" s="74"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="74" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="B23" s="110" t="s">
+        <v>140</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D23" s="74"/>
       <c r="E23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A24" s="73" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D24" s="74"/>
       <c r="E24" s="74"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="73" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D25" s="74"/>
       <c r="E25" s="74"/>
     </row>
     <row r="26" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A26" s="73" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B26" s="74" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D26" s="74"/>
       <c r="E26" s="74"/>

</xml_diff>

<commit_message>
Eliminación de imágenes de stock por exceso de peso
</commit_message>
<xml_diff>
--- a/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
+++ b/guiasYformatos/solicitudes/formatos/SolicitudGrafica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\RecursosGenerales\guiasYformatos\solicitudes\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\RecursosGenerales\guiasYformatos\solicitudes\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1210,7 +1210,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1275,29 +1275,8 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1418,6 +1397,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1503,9 +1485,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2355,12 +2334,12 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.5625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.1875" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="2" customWidth="1"/>
@@ -2383,8 +2362,8 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
@@ -2393,14 +2372,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
-      <c r="F2" s="79" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="F2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
@@ -2408,12 +2387,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="89"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
@@ -2421,15 +2400,15 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
@@ -2438,16 +2417,16 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="53" t="str">
+      <c r="F5" s="46" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
         <v/>
       </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="77"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="70"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
@@ -2459,20 +2438,20 @@
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="33" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="32" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="1"/>
@@ -2488,12 +2467,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2503,7 +2482,7 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="26.05" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -2518,16 +2497,16 @@
       <c r="E9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="69" t="s">
         <v>121</v>
       </c>
       <c r="J9" s="25" t="s">
@@ -2542,7 +2521,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v/>
       </c>
-      <c r="B10" s="27"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
@@ -2573,9 +2552,9 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v/>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="27" t="str">
-        <f t="shared" ref="C11:C22" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C11:C74" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D11" s="14"/>
@@ -2601,10 +2580,10 @@
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="str">
-        <f t="shared" ref="A12:A30" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="29"/>
+        <f t="shared" ref="A12:A75" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
+        <v/>
+      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2635,7 +2614,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2666,7 +2645,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2697,7 +2676,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2728,7 +2707,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2751,15 +2730,15 @@
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="37"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2790,7 +2769,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2818,10 +2797,10 @@
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B19" s="35"/>
+        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B19" s="13"/>
       <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2844,15 +2823,15 @@
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="37"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="30"/>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B20" s="28"/>
+        <f t="shared" ref="A20:A83" si="4">IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(LEFT(A19,3),IF(MID(A19,4,2)+1&lt;10,CONCATENATE("0",MID(A19,4,2)+1),MID(A19,4,2)+1)),"")</f>
+        <v/>
+      </c>
+      <c r="B20" s="13"/>
       <c r="C20" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2880,10 +2859,10 @@
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B21" s="30"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B21" s="13"/>
       <c r="C21" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2911,10 +2890,10 @@
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B22" s="31"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B22" s="13"/>
       <c r="C22" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2942,11 +2921,14 @@
     </row>
     <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="str">
@@ -2970,11 +2952,14 @@
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14" t="str">
@@ -2998,11 +2983,14 @@
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14" t="str">
@@ -3026,11 +3014,14 @@
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14" t="str">
@@ -3054,11 +3045,14 @@
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14" t="str">
@@ -3082,11 +3076,14 @@
     </row>
     <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14" t="str">
@@ -3110,11 +3107,14 @@
     </row>
     <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14" t="str">
@@ -3138,11 +3138,14 @@
     </row>
     <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14" t="str">
@@ -3165,9 +3168,15 @@
       <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14" t="str">
@@ -3190,9 +3199,15 @@
       <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14" t="str">
@@ -3215,9 +3230,15 @@
       <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14" t="str">
@@ -3240,9 +3261,15 @@
       <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14" t="str">
@@ -3265,9 +3292,15 @@
       <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
+      <c r="A35" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14" t="str">
@@ -3290,9 +3323,15 @@
       <c r="K35" s="15"/>
     </row>
     <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="A36" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14" t="str">
@@ -3315,9 +3354,15 @@
       <c r="K36" s="15"/>
     </row>
     <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="A37" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14" t="str">
@@ -3340,9 +3385,15 @@
       <c r="K37" s="15"/>
     </row>
     <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
+      <c r="A38" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14" t="str">
@@ -3365,9 +3416,15 @@
       <c r="K38" s="15"/>
     </row>
     <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
+      <c r="A39" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14" t="str">
@@ -3390,9 +3447,15 @@
       <c r="K39" s="15"/>
     </row>
     <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
+      <c r="A40" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14" t="str">
@@ -3415,9 +3478,15 @@
       <c r="K40" s="15"/>
     </row>
     <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
+      <c r="A41" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14" t="str">
@@ -3440,9 +3509,15 @@
       <c r="K41" s="15"/>
     </row>
     <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
+      <c r="A42" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="str">
@@ -3465,9 +3540,15 @@
       <c r="K42" s="15"/>
     </row>
     <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
+      <c r="A43" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14" t="str">
@@ -3490,9 +3571,15 @@
       <c r="K43" s="15"/>
     </row>
     <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14" t="str">
@@ -3515,9 +3602,15 @@
       <c r="K44" s="15"/>
     </row>
     <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14" t="str">
@@ -3540,9 +3633,15 @@
       <c r="K45" s="15"/>
     </row>
     <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14" t="str">
@@ -3565,9 +3664,15 @@
       <c r="K46" s="15"/>
     </row>
     <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
+      <c r="A47" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14" t="str">
@@ -3590,9 +3695,15 @@
       <c r="K47" s="15"/>
     </row>
     <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
+      <c r="A48" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14" t="str">
@@ -3615,9 +3726,15 @@
       <c r="K48" s="15"/>
     </row>
     <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
+      <c r="A49" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14" t="str">
@@ -3640,9 +3757,15 @@
       <c r="K49" s="15"/>
     </row>
     <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="13"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
+      <c r="A50" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14" t="str">
@@ -3665,9 +3788,15 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
+      <c r="A51" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14" t="str">
@@ -3690,9 +3819,15 @@
       <c r="K51" s="15"/>
     </row>
     <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
+      <c r="A52" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14" t="str">
@@ -3715,9 +3850,15 @@
       <c r="K52" s="15"/>
     </row>
     <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="13"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
+      <c r="A53" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14" t="str">
@@ -3740,9 +3881,15 @@
       <c r="K53" s="15"/>
     </row>
     <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
+      <c r="A54" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14" t="str">
@@ -3765,9 +3912,15 @@
       <c r="K54" s="15"/>
     </row>
     <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="13"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
+      <c r="A55" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14" t="str">
@@ -3790,9 +3943,15 @@
       <c r="K55" s="15"/>
     </row>
     <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
+      <c r="A56" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14" t="str">
@@ -3815,9 +3974,15 @@
       <c r="K56" s="15"/>
     </row>
     <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="13"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
+      <c r="A57" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14" t="str">
@@ -3840,9 +4005,15 @@
       <c r="K57" s="15"/>
     </row>
     <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="13"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
+      <c r="A58" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14" t="str">
@@ -3865,9 +4036,15 @@
       <c r="K58" s="15"/>
     </row>
     <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
+      <c r="A59" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14" t="str">
@@ -3890,9 +4067,15 @@
       <c r="K59" s="15"/>
     </row>
     <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
+      <c r="A60" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14" t="str">
@@ -3915,9 +4098,15 @@
       <c r="K60" s="15"/>
     </row>
     <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="13"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
+      <c r="A61" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14" t="str">
@@ -3940,9 +4129,15 @@
       <c r="K61" s="15"/>
     </row>
     <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13"/>
+      <c r="A62" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
+      <c r="C62" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14" t="str">
@@ -3965,9 +4160,15 @@
       <c r="K62" s="15"/>
     </row>
     <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="13"/>
+      <c r="A63" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
+      <c r="C63" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14" t="str">
@@ -3990,9 +4191,15 @@
       <c r="K63" s="15"/>
     </row>
     <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="13"/>
+      <c r="A64" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
+      <c r="C64" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14" t="str">
@@ -4015,9 +4222,15 @@
       <c r="K64" s="15"/>
     </row>
     <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="13"/>
+      <c r="A65" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
+      <c r="C65" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="14" t="str">
@@ -4040,9 +4253,15 @@
       <c r="K65" s="15"/>
     </row>
     <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="13"/>
+      <c r="A66" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
+      <c r="C66" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14" t="str">
@@ -4065,9 +4284,15 @@
       <c r="K66" s="15"/>
     </row>
     <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="13"/>
+      <c r="A67" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
+      <c r="C67" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14" t="str">
@@ -4090,9 +4315,15 @@
       <c r="K67" s="15"/>
     </row>
     <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="13"/>
+      <c r="A68" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
+      <c r="C68" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14" t="str">
@@ -4115,9 +4346,15 @@
       <c r="K68" s="15"/>
     </row>
     <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="13"/>
+      <c r="A69" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="C69" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14" t="str">
@@ -4140,9 +4377,15 @@
       <c r="K69" s="15"/>
     </row>
     <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="13"/>
+      <c r="A70" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="C70" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14" t="str">
@@ -4165,9 +4408,15 @@
       <c r="K70" s="15"/>
     </row>
     <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="13"/>
+      <c r="A71" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
+      <c r="C71" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14" t="str">
@@ -4190,9 +4439,15 @@
       <c r="K71" s="15"/>
     </row>
     <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="13"/>
+      <c r="A72" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
+      <c r="C72" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14" t="str">
@@ -4215,9 +4470,15 @@
       <c r="K72" s="15"/>
     </row>
     <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="13"/>
+      <c r="A73" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
+      <c r="C73" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14" t="str">
@@ -4240,9 +4501,15 @@
       <c r="K73" s="15"/>
     </row>
     <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="13"/>
+      <c r="A74" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
+      <c r="C74" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14" t="str">
@@ -4265,13 +4532,19 @@
       <c r="K74" s="15"/>
     </row>
     <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="13"/>
+      <c r="A75" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
+      <c r="C75" s="27" t="str">
+        <f t="shared" ref="C75:C108" si="5">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v/>
+      </c>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="14" t="str">
-        <f t="shared" ref="F75:F108" si="4">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F75:F108" si="6">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G75" s="14" t="str">
@@ -4279,7 +4552,7 @@
         <v/>
       </c>
       <c r="H75" s="14" t="str">
-        <f t="shared" ref="H75:H108" si="5">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H75:H108" si="7">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I75" s="14" t="str">
@@ -4290,13 +4563,19 @@
       <c r="K75" s="15"/>
     </row>
     <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="13"/>
+      <c r="A76" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
+      <c r="C76" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G76" s="14" t="str">
@@ -4304,7 +4583,7 @@
         <v/>
       </c>
       <c r="H76" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I76" s="14" t="str">
@@ -4315,13 +4594,19 @@
       <c r="K76" s="15"/>
     </row>
     <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="13"/>
+      <c r="A77" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="C77" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G77" s="14" t="str">
@@ -4329,7 +4614,7 @@
         <v/>
       </c>
       <c r="H77" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I77" s="14" t="str">
@@ -4340,13 +4625,19 @@
       <c r="K77" s="15"/>
     </row>
     <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="13"/>
+      <c r="A78" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
+      <c r="C78" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G78" s="14" t="str">
@@ -4354,7 +4645,7 @@
         <v/>
       </c>
       <c r="H78" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I78" s="14" t="str">
@@ -4365,13 +4656,19 @@
       <c r="K78" s="15"/>
     </row>
     <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="13"/>
+      <c r="A79" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
+      <c r="C79" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G79" s="14" t="str">
@@ -4379,7 +4676,7 @@
         <v/>
       </c>
       <c r="H79" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I79" s="14" t="str">
@@ -4390,13 +4687,19 @@
       <c r="K79" s="15"/>
     </row>
     <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="13"/>
+      <c r="A80" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="C80" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G80" s="14" t="str">
@@ -4404,7 +4707,7 @@
         <v/>
       </c>
       <c r="H80" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I80" s="14" t="str">
@@ -4415,13 +4718,19 @@
       <c r="K80" s="15"/>
     </row>
     <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="13"/>
+      <c r="A81" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="C81" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G81" s="14" t="str">
@@ -4429,7 +4738,7 @@
         <v/>
       </c>
       <c r="H81" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I81" s="14" t="str">
@@ -4440,13 +4749,19 @@
       <c r="K81" s="15"/>
     </row>
     <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="13"/>
+      <c r="A82" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="C82" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G82" s="14" t="str">
@@ -4454,7 +4769,7 @@
         <v/>
       </c>
       <c r="H82" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I82" s="14" t="str">
@@ -4465,13 +4780,19 @@
       <c r="K82" s="15"/>
     </row>
     <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="13"/>
+      <c r="A83" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="C83" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G83" s="14" t="str">
@@ -4479,7 +4800,7 @@
         <v/>
       </c>
       <c r="H83" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I83" s="14" t="str">
@@ -4490,13 +4811,19 @@
       <c r="K83" s="15"/>
     </row>
     <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="13"/>
+      <c r="A84" s="13" t="str">
+        <f t="shared" ref="A84:A108" si="8">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
+        <v/>
+      </c>
       <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="C84" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G84" s="14" t="str">
@@ -4504,7 +4831,7 @@
         <v/>
       </c>
       <c r="H84" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I84" s="14" t="str">
@@ -4515,13 +4842,19 @@
       <c r="K84" s="15"/>
     </row>
     <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="13"/>
+      <c r="A85" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
+      <c r="C85" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G85" s="14" t="str">
@@ -4529,7 +4862,7 @@
         <v/>
       </c>
       <c r="H85" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I85" s="14" t="str">
@@ -4540,13 +4873,19 @@
       <c r="K85" s="15"/>
     </row>
     <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="13"/>
+      <c r="A86" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
+      <c r="C86" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G86" s="14" t="str">
@@ -4554,7 +4893,7 @@
         <v/>
       </c>
       <c r="H86" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I86" s="14" t="str">
@@ -4565,13 +4904,19 @@
       <c r="K86" s="15"/>
     </row>
     <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="13"/>
+      <c r="A87" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
+      <c r="C87" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G87" s="14" t="str">
@@ -4579,7 +4924,7 @@
         <v/>
       </c>
       <c r="H87" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I87" s="14" t="str">
@@ -4590,13 +4935,19 @@
       <c r="K87" s="15"/>
     </row>
     <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="13"/>
+      <c r="A88" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
+      <c r="C88" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G88" s="14" t="str">
@@ -4604,7 +4955,7 @@
         <v/>
       </c>
       <c r="H88" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I88" s="14" t="str">
@@ -4615,13 +4966,19 @@
       <c r="K88" s="15"/>
     </row>
     <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="13"/>
+      <c r="A89" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
+      <c r="C89" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G89" s="14" t="str">
@@ -4629,7 +4986,7 @@
         <v/>
       </c>
       <c r="H89" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I89" s="14" t="str">
@@ -4640,13 +4997,19 @@
       <c r="K89" s="15"/>
     </row>
     <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="13"/>
+      <c r="A90" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="C90" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G90" s="14" t="str">
@@ -4654,7 +5017,7 @@
         <v/>
       </c>
       <c r="H90" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I90" s="14" t="str">
@@ -4665,13 +5028,19 @@
       <c r="K90" s="15"/>
     </row>
     <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="13"/>
+      <c r="A91" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="C91" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G91" s="14" t="str">
@@ -4679,7 +5048,7 @@
         <v/>
       </c>
       <c r="H91" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I91" s="14" t="str">
@@ -4690,13 +5059,19 @@
       <c r="K91" s="15"/>
     </row>
     <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="13"/>
+      <c r="A92" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="C92" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G92" s="14" t="str">
@@ -4704,7 +5079,7 @@
         <v/>
       </c>
       <c r="H92" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I92" s="14" t="str">
@@ -4715,13 +5090,19 @@
       <c r="K92" s="15"/>
     </row>
     <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="13"/>
+      <c r="A93" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="C93" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G93" s="14" t="str">
@@ -4729,7 +5110,7 @@
         <v/>
       </c>
       <c r="H93" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I93" s="14" t="str">
@@ -4740,13 +5121,19 @@
       <c r="K93" s="15"/>
     </row>
     <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="13"/>
+      <c r="A94" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="C94" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G94" s="14" t="str">
@@ -4754,7 +5141,7 @@
         <v/>
       </c>
       <c r="H94" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I94" s="14" t="str">
@@ -4765,13 +5152,19 @@
       <c r="K94" s="15"/>
     </row>
     <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="13"/>
+      <c r="A95" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="C95" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G95" s="14" t="str">
@@ -4779,7 +5172,7 @@
         <v/>
       </c>
       <c r="H95" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I95" s="14" t="str">
@@ -4790,13 +5183,19 @@
       <c r="K95" s="15"/>
     </row>
     <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="13"/>
+      <c r="A96" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="C96" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G96" s="14" t="str">
@@ -4804,7 +5203,7 @@
         <v/>
       </c>
       <c r="H96" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I96" s="14" t="str">
@@ -4815,13 +5214,19 @@
       <c r="K96" s="15"/>
     </row>
     <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="13"/>
+      <c r="A97" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="C97" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G97" s="14" t="str">
@@ -4829,7 +5234,7 @@
         <v/>
       </c>
       <c r="H97" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I97" s="14" t="str">
@@ -4840,13 +5245,19 @@
       <c r="K97" s="15"/>
     </row>
     <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="13"/>
+      <c r="A98" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="C98" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G98" s="14" t="str">
@@ -4854,7 +5265,7 @@
         <v/>
       </c>
       <c r="H98" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I98" s="14" t="str">
@@ -4865,13 +5276,19 @@
       <c r="K98" s="15"/>
     </row>
     <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="13"/>
+      <c r="A99" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="C99" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
       <c r="F99" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G99" s="14" t="str">
@@ -4879,7 +5296,7 @@
         <v/>
       </c>
       <c r="H99" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I99" s="14" t="str">
@@ -4890,13 +5307,19 @@
       <c r="K99" s="15"/>
     </row>
     <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="13"/>
+      <c r="A100" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="C100" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
       <c r="F100" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G100" s="14" t="str">
@@ -4904,7 +5327,7 @@
         <v/>
       </c>
       <c r="H100" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I100" s="14" t="str">
@@ -4915,13 +5338,19 @@
       <c r="K100" s="15"/>
     </row>
     <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="13"/>
+      <c r="A101" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="C101" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G101" s="14" t="str">
@@ -4929,7 +5358,7 @@
         <v/>
       </c>
       <c r="H101" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I101" s="14" t="str">
@@ -4940,13 +5369,19 @@
       <c r="K101" s="15"/>
     </row>
     <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="13"/>
+      <c r="A102" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="C102" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G102" s="14" t="str">
@@ -4954,7 +5389,7 @@
         <v/>
       </c>
       <c r="H102" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I102" s="14" t="str">
@@ -4965,13 +5400,19 @@
       <c r="K102" s="15"/>
     </row>
     <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="13"/>
+      <c r="A103" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
+      <c r="C103" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
       <c r="F103" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G103" s="14" t="str">
@@ -4979,7 +5420,7 @@
         <v/>
       </c>
       <c r="H103" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I103" s="14" t="str">
@@ -4990,13 +5431,19 @@
       <c r="K103" s="15"/>
     </row>
     <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="13"/>
+      <c r="A104" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
+      <c r="C104" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
       <c r="F104" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G104" s="14" t="str">
@@ -5004,7 +5451,7 @@
         <v/>
       </c>
       <c r="H104" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I104" s="14" t="str">
@@ -5015,13 +5462,19 @@
       <c r="K104" s="15"/>
     </row>
     <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="13"/>
+      <c r="A105" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
+      <c r="C105" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
       <c r="F105" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G105" s="14" t="str">
@@ -5029,7 +5482,7 @@
         <v/>
       </c>
       <c r="H105" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I105" s="14" t="str">
@@ -5040,13 +5493,19 @@
       <c r="K105" s="15"/>
     </row>
     <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="13"/>
+      <c r="A106" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B106" s="13"/>
-      <c r="C106" s="13"/>
+      <c r="C106" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
       <c r="F106" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G106" s="14" t="str">
@@ -5054,7 +5513,7 @@
         <v/>
       </c>
       <c r="H106" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I106" s="14" t="str">
@@ -5065,13 +5524,19 @@
       <c r="K106" s="15"/>
     </row>
     <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="13"/>
+      <c r="A107" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
+      <c r="C107" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
       <c r="F107" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G107" s="14" t="str">
@@ -5079,7 +5544,7 @@
         <v/>
       </c>
       <c r="H107" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I107" s="14" t="str">
@@ -5090,13 +5555,19 @@
       <c r="K107" s="15"/>
     </row>
     <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="13"/>
+      <c r="A108" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
+      <c r="C108" s="27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
       <c r="F108" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G108" s="14" t="str">
@@ -5104,7 +5575,7 @@
         <v/>
       </c>
       <c r="H108" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I108" s="14" t="str">
@@ -5182,539 +5653,539 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="38" customWidth="1"/>
-    <col min="2" max="2" width="11" style="38"/>
-    <col min="3" max="3" width="13.8125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" style="38" customWidth="1"/>
-    <col min="5" max="7" width="11" style="38"/>
-    <col min="8" max="11" width="11" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="38"/>
+    <col min="1" max="1" width="72.25" style="31" customWidth="1"/>
+    <col min="2" max="2" width="11" style="31"/>
+    <col min="3" max="3" width="13.8125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" style="31" customWidth="1"/>
+    <col min="5" max="7" width="11" style="31"/>
+    <col min="8" max="11" width="11" style="31" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="90"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="97" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="48"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="103" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="48"/>
-      <c r="H3" s="38" t="s">
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="41"/>
+      <c r="H3" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="H4" s="38" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="31">
         <v>1</v>
       </c>
-      <c r="K4" s="38">
+      <c r="K4" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="44" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="106" t="str">
+      <c r="D5" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="48"/>
-      <c r="H5" s="38" t="s">
+      <c r="E5" s="101"/>
+      <c r="F5" s="41"/>
+      <c r="H5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="31">
         <v>2</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
-      <c r="H6" s="38" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="H6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="31">
         <v>3</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="31">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="78" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="92" t="str">
+      <c r="D7" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
-      <c r="H7" s="38" t="s">
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
+      <c r="H7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="31">
         <v>4</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="I8" s="38" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="I8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="31">
         <v>5</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="I9" s="38" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="I9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="31">
         <v>6</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
-      <c r="I10" s="38" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="I10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="31">
         <v>7</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="38">
+      <c r="J11" s="31">
         <v>8</v>
       </c>
-      <c r="K11" s="38">
+      <c r="K11" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="31">
         <v>9</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="31">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96"/>
-      <c r="I13" s="38" t="s">
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
+      <c r="I13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="38">
+      <c r="J13" s="31">
         <v>10</v>
       </c>
-      <c r="K13" s="38">
+      <c r="K13" s="31">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="49"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="I14" s="38" t="s">
+      <c r="A14" s="42"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="I14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="38">
+      <c r="J14" s="31">
         <v>11</v>
       </c>
-      <c r="K14" s="38">
+      <c r="K14" s="31">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="97" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
-      <c r="J15" s="38">
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="93"/>
+      <c r="J15" s="31">
         <v>12</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="31">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="67.099999999999994" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="42" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="38">
+      <c r="J16" s="31">
         <v>13</v>
       </c>
-      <c r="K16" s="38">
+      <c r="K16" s="31">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="44" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="100" t="str">
+      <c r="D17" s="94" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
-      <c r="J17" s="38">
+      <c r="E17" s="95"/>
+      <c r="F17" s="96"/>
+      <c r="J17" s="31">
         <v>14</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="31">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="78" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="92" t="str">
+      <c r="D18" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="93"/>
-      <c r="J18" s="38">
+      <c r="E18" s="86"/>
+      <c r="F18" s="87"/>
+      <c r="J18" s="31">
         <v>15</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="31">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="H19" s="38">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="H19" s="31">
         <v>3</v>
       </c>
-      <c r="J19" s="38">
+      <c r="J19" s="31">
         <v>16</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="31">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-      <c r="H20" s="38">
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
+      <c r="H20" s="31">
         <v>4</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="31">
         <v>5</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J20" s="31">
         <v>4</v>
       </c>
-      <c r="K20" s="38">
+      <c r="K20" s="31">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="H21" s="38" t="str">
+      <c r="H21" s="31" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
       </c>
-      <c r="I21" s="38" t="str">
+      <c r="I21" s="31" t="str">
         <f>CONCATENATE(IF((I20+2)&lt;10,"0",""),I20+2)</f>
         <v>07</v>
       </c>
-      <c r="J21" s="38" t="str">
+      <c r="J21" s="31" t="str">
         <f>CONCATENATE(IF(J20&lt;10,"0",""),J20)</f>
         <v>04</v>
       </c>
-      <c r="K21" s="38">
+      <c r="K21" s="31">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K22" s="38">
+      <c r="K22" s="31">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K23" s="38">
+      <c r="K23" s="31">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K24" s="38">
+      <c r="K24" s="31">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K25" s="38">
+      <c r="K25" s="31">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K26" s="38">
+      <c r="K26" s="31">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K27" s="38">
+      <c r="K27" s="31">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K28" s="38">
+      <c r="K28" s="31">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K29" s="38">
+      <c r="K29" s="31">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K30" s="38">
+      <c r="K30" s="31">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K31" s="38">
+      <c r="K31" s="31">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="K32" s="38">
+      <c r="K32" s="31">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K33" s="38">
+      <c r="K33" s="31">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K34" s="38">
+      <c r="K34" s="31">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K35" s="38">
+      <c r="K35" s="31">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K36" s="38">
+      <c r="K36" s="31">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K37" s="38">
+      <c r="K37" s="31">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K38" s="38">
+      <c r="K38" s="31">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K39" s="38">
+      <c r="K39" s="31">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K40" s="38">
+      <c r="K40" s="31">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K41" s="38">
+      <c r="K41" s="31">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K42" s="38">
+      <c r="K42" s="31">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K43" s="38">
+      <c r="K43" s="31">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K44" s="38">
+      <c r="K44" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K45" s="38" t="str">
+      <c r="K45" s="31" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
       </c>
@@ -5909,562 +6380,562 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8125" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="21" style="38" customWidth="1"/>
-    <col min="2" max="2" width="22.1875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="17.3125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="10.8125" style="38"/>
-    <col min="5" max="5" width="11.6875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="12.6875" style="38" customWidth="1"/>
-    <col min="7" max="7" width="11" style="38" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="38" customWidth="1"/>
-    <col min="9" max="9" width="22.1875" style="38" customWidth="1"/>
-    <col min="10" max="10" width="20.6875" style="38" customWidth="1"/>
-    <col min="11" max="11" width="44.5" style="38" customWidth="1"/>
-    <col min="12" max="16384" width="10.8125" style="38"/>
+    <col min="1" max="1" width="21" style="31" customWidth="1"/>
+    <col min="2" max="2" width="22.1875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="17.3125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="10.8125" style="31"/>
+    <col min="5" max="5" width="11.6875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="12.6875" style="31" customWidth="1"/>
+    <col min="7" max="7" width="11" style="31" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="31" customWidth="1"/>
+    <col min="9" max="9" width="22.1875" style="31" customWidth="1"/>
+    <col min="10" max="10" width="20.6875" style="31" customWidth="1"/>
+    <col min="11" max="11" width="44.5" style="31" customWidth="1"/>
+    <col min="12" max="16384" width="10.8125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="57" t="s">
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="50" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="58" t="s">
+    <row r="3" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-    </row>
-    <row r="4" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="60" t="s">
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60" t="s">
+      <c r="G4" s="53"/>
+      <c r="H4" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J4" s="60"/>
-    </row>
-    <row r="5" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="61" t="s">
+      <c r="J4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="62"/>
-      <c r="H5" s="60" t="s">
+      <c r="G5" s="55"/>
+      <c r="H5" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="62"/>
-    </row>
-    <row r="6" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="60" t="s">
+      <c r="J5" s="55"/>
+    </row>
+    <row r="6" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="53" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A7" s="60" t="s">
+    <row r="7" spans="1:11" s="52" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A7" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60" t="s">
+      <c r="G7" s="53"/>
+      <c r="H7" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J7" s="60"/>
-    </row>
-    <row r="8" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="60" t="s">
+      <c r="J7" s="53"/>
+    </row>
+    <row r="8" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60" t="s">
+      <c r="G8" s="53"/>
+      <c r="H8" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J8" s="60"/>
-    </row>
-    <row r="9" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="60" t="s">
+      <c r="J8" s="53"/>
+    </row>
+    <row r="9" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60" t="s">
+      <c r="G9" s="53"/>
+      <c r="H9" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J9" s="60"/>
-    </row>
-    <row r="10" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="60" t="s">
+      <c r="J9" s="53"/>
+    </row>
+    <row r="10" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60" t="s">
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J10" s="60"/>
-    </row>
-    <row r="11" spans="1:11" s="59" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A11" s="60" t="s">
+      <c r="J10" s="53"/>
+    </row>
+    <row r="11" spans="1:11" s="52" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A11" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60" t="s">
+      <c r="G11" s="53"/>
+      <c r="H11" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J11" s="60"/>
-    </row>
-    <row r="12" spans="1:11" s="59" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="60" t="s">
+      <c r="J11" s="53"/>
+    </row>
+    <row r="12" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60" t="s">
+      <c r="G12" s="53"/>
+      <c r="H12" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I12" s="60" t="s">
+      <c r="I12" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J12" s="60"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65" t="s">
+      <c r="E13" s="57"/>
+      <c r="F13" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="63"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60" t="s">
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="38" t="s">
+      <c r="J13" s="56"/>
+      <c r="K13" s="31" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65" t="s">
+      <c r="E14" s="57"/>
+      <c r="F14" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="63"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60" t="s">
+      <c r="G14" s="56"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="J14" s="63"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="60" t="s">
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="38" t="s">
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="31" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="95" x14ac:dyDescent="0.5">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="61" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="D16" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="64"/>
-      <c r="H16" s="65" t="s">
+      <c r="G16" s="57"/>
+      <c r="H16" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="I16" s="65" t="s">
+      <c r="I16" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="J16" s="64"/>
-      <c r="K16" s="66" t="s">
+      <c r="J16" s="57"/>
+      <c r="K16" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="67" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="60"/>
-      <c r="K17" s="68" t="s">
+      <c r="J17" s="53"/>
+      <c r="K17" s="61" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="62" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="110" t="s">
+      <c r="B23" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
     </row>
     <row r="24" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="68" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
     </row>
     <row r="26" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>